<commit_message>
finish evaluating on model svm sift
</commit_message>
<xml_diff>
--- a/Skripsi/Parameter Tuning.xlsx
+++ b/Skripsi/Parameter Tuning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GDrive\Skripsi\Repos\Skripsi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943DF94E-A587-49EB-B79E-720FC7D38A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F7E616-56FA-4736-98DD-AD9C201D1BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="15">
   <si>
     <t>Resize</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>['auto', 0.0024, 0.0032, 0.0048, 0.0056]</t>
+  </si>
+  <si>
+    <t>Kesimpulan</t>
   </si>
 </sst>
 </file>
@@ -212,11 +215,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -285,6 +285,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -302,6 +314,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>290272</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>114556</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B587421-4152-4EFF-BBFC-86FC5CEDF7B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7200900" y="708660"/>
+          <a:ext cx="8215072" cy="2949196"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -567,372 +628,515 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="1"/>
-    <col min="3" max="3" width="15.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="41.6640625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="10.6640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="2" width="8.88671875" style="7"/>
+    <col min="3" max="3" width="15.33203125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="41.6640625" style="7" customWidth="1"/>
+    <col min="5" max="6" width="10.6640625" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="8" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="8" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13">
+    <row r="2" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12">
         <v>128</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>180</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="9">
         <v>0.90229999999999999</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="9">
         <v>0.9274</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="8" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="2">
+    <row r="3" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="13"/>
+      <c r="B3" s="1">
         <v>250</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="13"/>
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="9">
         <v>0.90869999999999995</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="9">
         <v>0.92510000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="8" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="2">
+    <row r="4" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13"/>
+      <c r="B4" s="1">
         <v>500</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="2" t="s">
+      <c r="C4" s="13"/>
+      <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="9">
         <v>0.92349999999999999</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="9">
         <v>0.94779999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="8" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
-      <c r="B5" s="2">
+    <row r="5" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="13"/>
+      <c r="B5" s="1">
         <v>750</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="2" t="s">
+      <c r="C5" s="13"/>
+      <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <v>0.93069999999999997</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="9">
         <v>0.95230000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="8" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
-      <c r="B6" s="2">
+    <row r="6" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="14"/>
+      <c r="B6" s="1">
         <v>1000</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-    </row>
-    <row r="7" spans="1:9" s="8" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16">
+      <c r="E6" s="9">
+        <v>0.92230000000000001</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0.94550000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="15">
         <v>160</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>180</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="10">
         <v>0.89229999999999998</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="10">
         <v>0.90920000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="8" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
-      <c r="B8" s="3">
+    <row r="8" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="16"/>
+      <c r="B8" s="2">
         <v>250</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="3" t="s">
+      <c r="C8" s="16"/>
+      <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="10">
         <v>0.90790000000000004</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="10">
         <v>0.95009999999999994</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="8" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
-      <c r="B9" s="3">
+    <row r="9" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="16"/>
+      <c r="B9" s="2">
         <v>500</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="3" t="s">
+      <c r="C9" s="16"/>
+      <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="10">
         <v>0.91710000000000003</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="10">
         <v>0.93869999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="8" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17"/>
-      <c r="B10" s="3">
+    <row r="10" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="16"/>
+      <c r="B10" s="2">
         <v>750</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="3" t="s">
+      <c r="C10" s="16"/>
+      <c r="D10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="10">
         <v>0.91669999999999996</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="10">
         <v>0.94779999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="8" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18"/>
-      <c r="B11" s="3">
+    <row r="11" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="17"/>
+      <c r="B11" s="2">
         <v>1000</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="3" t="s">
+      <c r="C11" s="17"/>
+      <c r="D11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-    </row>
-    <row r="12" spans="1:9" s="8" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19">
+      <c r="E11" s="10">
+        <v>0.92390000000000005</v>
+      </c>
+      <c r="F11" s="10">
+        <v>0.9365</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="18">
         <v>192</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>180</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>0.89390000000000003</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <v>0.92510000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="8" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="20"/>
-      <c r="B13" s="4">
+    <row r="13" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="19"/>
+      <c r="B13" s="3">
         <v>250</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="4" t="s">
+      <c r="C13" s="19"/>
+      <c r="D13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>0.90590000000000004</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="5">
         <v>0.9274</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="8" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="20"/>
-      <c r="B14" s="4">
+    <row r="14" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="19"/>
+      <c r="B14" s="3">
         <v>500</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="4" t="s">
+      <c r="C14" s="19"/>
+      <c r="D14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <v>0.91749999999999998</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="5">
         <v>0.94550000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="8" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="20"/>
-      <c r="B15" s="4">
+    <row r="15" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="19"/>
+      <c r="B15" s="3">
         <v>750</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="4" t="s">
+      <c r="C15" s="19"/>
+      <c r="D15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <v>0.92349999999999999</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="5">
         <v>0.9546</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="8" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21"/>
-      <c r="B16" s="4">
+    <row r="16" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="20"/>
+      <c r="B16" s="3">
         <v>1000</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="4" t="s">
+      <c r="C16" s="20"/>
+      <c r="D16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="1:6" s="8" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="22">
+      <c r="E16" s="5">
+        <v>0.93469999999999998</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.94550000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="21">
         <v>224</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="4">
         <v>180</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="11">
         <v>0.87070000000000003</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="11">
         <v>0.91379999999999995</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" s="8" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="23"/>
-      <c r="B18" s="5">
+      <c r="H17" s="27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="22"/>
+      <c r="B18" s="4">
         <v>250</v>
       </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="5" t="s">
+      <c r="C18" s="22"/>
+      <c r="D18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="11">
         <v>0.87350000000000005</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="11">
         <v>0.90920000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="8" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="23"/>
-      <c r="B19" s="5">
+    <row r="19" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="22"/>
+      <c r="B19" s="4">
         <v>500</v>
       </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="5" t="s">
+      <c r="C19" s="22"/>
+      <c r="D19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="11">
         <v>0.90910000000000002</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19" s="11">
         <v>0.94330000000000003</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" s="8" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="23"/>
-      <c r="B20" s="5">
+      <c r="H19" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="I19" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="J19" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="L19" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="M19" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="N19" s="24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="22"/>
+      <c r="B20" s="4">
         <v>750</v>
       </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="5" t="s">
+      <c r="C20" s="22"/>
+      <c r="D20" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-    </row>
-    <row r="21" spans="1:6" s="8" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="24"/>
-      <c r="B21" s="5">
+      <c r="E20" s="11">
+        <v>0.92149999999999999</v>
+      </c>
+      <c r="F20" s="11">
+        <v>0.93189999999999995</v>
+      </c>
+      <c r="H20" s="25">
+        <v>128</v>
+      </c>
+      <c r="I20" s="26">
+        <f>AVERAGE(E2:E6)</f>
+        <v>0.91749999999999987</v>
+      </c>
+      <c r="J20" s="26">
+        <f>AVERAGE(F2:F6)</f>
+        <v>0.93962000000000001</v>
+      </c>
+      <c r="L20" s="25">
+        <v>180</v>
+      </c>
+      <c r="M20" s="26">
+        <f>AVERAGE(E2,E7,E12,E17)</f>
+        <v>0.88979999999999992</v>
+      </c>
+      <c r="N20" s="26">
+        <f>AVERAGE(F2,F7,F12,F17)</f>
+        <v>0.91887500000000011</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="23"/>
+      <c r="B21" s="4">
         <v>1000</v>
       </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="5" t="s">
+      <c r="C21" s="23"/>
+      <c r="D21" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-    </row>
-    <row r="22" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="E21" s="11">
+        <v>0.92430000000000001</v>
+      </c>
+      <c r="F21" s="11">
+        <v>0.95009999999999994</v>
+      </c>
+      <c r="H21" s="25">
+        <v>160</v>
+      </c>
+      <c r="I21" s="26">
+        <f>AVERAGE(E7:E11)</f>
+        <v>0.91158000000000006</v>
+      </c>
+      <c r="J21" s="26">
+        <f>AVERAGE(F7:F11)</f>
+        <v>0.93645999999999996</v>
+      </c>
+      <c r="L21" s="25">
+        <v>250</v>
+      </c>
+      <c r="M21" s="26">
+        <f>AVERAGE(E3,E8,E13,E18)</f>
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="N21" s="26">
+        <f>AVERAGE(F3,F8,F13,F18)</f>
+        <v>0.92795000000000005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H22" s="25">
+        <v>192</v>
+      </c>
+      <c r="I22" s="26">
+        <f>AVERAGE(E12:E16)</f>
+        <v>0.91510000000000002</v>
+      </c>
+      <c r="J22" s="26">
+        <f>AVERAGE(F12:F16)</f>
+        <v>0.93962000000000001</v>
+      </c>
+      <c r="L22" s="25">
+        <v>500</v>
+      </c>
+      <c r="M22" s="26">
+        <f>AVERAGE(E4,E9,E14,E19)</f>
+        <v>0.91679999999999995</v>
+      </c>
+      <c r="N22" s="26">
+        <f>AVERAGE(F4,F9,F14,F19)</f>
+        <v>0.94382499999999991</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H23" s="25">
+        <v>224</v>
+      </c>
+      <c r="I23" s="26">
+        <f>AVERAGE(E17:E21)</f>
+        <v>0.89982000000000006</v>
+      </c>
+      <c r="J23" s="26">
+        <f>AVERAGE(F17:F21)</f>
+        <v>0.92965999999999993</v>
+      </c>
+      <c r="L23" s="25">
+        <v>750</v>
+      </c>
+      <c r="M23" s="26">
+        <f>AVERAGE(E5,E10,E15,E20)</f>
+        <v>0.92310000000000003</v>
+      </c>
+      <c r="N23" s="26">
+        <f>AVERAGE(F5,F10,F15,F20)</f>
+        <v>0.94664999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L24" s="25">
+        <v>1000</v>
+      </c>
+      <c r="M24" s="26">
+        <f>AVERAGE(E6,E11,E16,E21)</f>
+        <v>0.92630000000000001</v>
+      </c>
+      <c r="N24" s="26">
+        <f>AVERAGE(F6,F11,F16,F21)</f>
+        <v>0.94440000000000002</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A2:A6"/>
@@ -946,5 +1150,9 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="I20:J21 I22:I23 J22:J23" formulaRange="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>